<commit_message>
More work on getting the state machine coded up
</commit_message>
<xml_diff>
--- a/doc/systems/Beaglebone States.xlsx
+++ b/doc/systems/Beaglebone States.xlsx
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Finished implementing the state machine states
</commit_message>
<xml_diff>
--- a/doc/systems/Beaglebone States.xlsx
+++ b/doc/systems/Beaglebone States.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="70">
   <si>
     <t>State</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t xml:space="preserve">Shore commands a self test to determine in all faults are clear. </t>
+  </si>
+  <si>
+    <t>Signal restored, last state Armed</t>
+  </si>
+  <si>
+    <t>Shore commands WaypointNavigation state</t>
+  </si>
+  <si>
+    <t>Shore commands Manual state</t>
   </si>
 </sst>
 </file>
@@ -755,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,7 +1377,7 @@
         <v>37</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1466,7 +1475,7 @@
         <v>37</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1474,13 +1483,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1491,10 +1500,10 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1502,13 +1511,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1519,10 +1528,10 @@
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1533,37 +1542,51 @@
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
         <v>6</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
         <v>4</v>
       </c>
-      <c r="C57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More master control compilation
</commit_message>
<xml_diff>
--- a/doc/systems/Beaglebone States.xlsx
+++ b/doc/systems/Beaglebone States.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="70">
   <si>
     <t>State</t>
   </si>
@@ -764,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,6 +1590,39 @@
         <v>66</v>
       </c>
     </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>